<commit_message>
Minor Bug fixes to tables and data, improved ERD
</commit_message>
<xml_diff>
--- a/VectorDataInExcel-3NF.xlsx
+++ b/VectorDataInExcel-3NF.xlsx
@@ -999,8 +999,8 @@
   </sheetPr>
   <dimension ref="A2:G73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="F45" sqref="F45"/>
+    <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="40.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated Db to reflect new info
</commit_message>
<xml_diff>
--- a/VectorDataInExcel-3NF.xlsx
+++ b/VectorDataInExcel-3NF.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nick\OneDrive - Ara Institute of Canterbury\Year 2\Semester 1\Database\Assignment1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="479" documentId="8_{9B9F850F-ADFF-4EEF-A28E-9D797F0D7DC6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{1737A932-8D2D-41B6-8798-BBB60CF92DB5}"/>
+  <xr:revisionPtr revIDLastSave="484" documentId="8_{9B9F850F-ADFF-4EEF-A28E-9D797F0D7DC6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{90CDA97A-48B6-4072-9CED-136863BE4F78}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{7DCE2BE0-953A-4365-ADEC-B2ECAC53B523}"/>
   </bookViews>
@@ -999,8 +999,8 @@
   </sheetPr>
   <dimension ref="A2:G74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="G68" sqref="G68"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+      <selection activeCell="G67" sqref="G67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="40.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2166,71 +2166,71 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B64" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C64" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="D64" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="E64" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="F64" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="G64" s="32" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B65" s="10">
+        <v>3.92</v>
+      </c>
+      <c r="C65" s="32">
+        <v>3.92</v>
+      </c>
+      <c r="D65" s="32">
+        <v>3.88</v>
+      </c>
+      <c r="E65" s="32">
+        <v>3.94</v>
+      </c>
+      <c r="F65" s="32">
+        <v>3.69</v>
+      </c>
+      <c r="G65" s="32">
+        <v>3.88</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="B64" s="6" t="s">
+      <c r="B67" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="C64" s="32" t="s">
+      <c r="C67" s="32" t="s">
         <v>137</v>
       </c>
-      <c r="D64" s="32" t="s">
+      <c r="D67" s="32" t="s">
         <v>138</v>
       </c>
-      <c r="E64" s="32" t="s">
+      <c r="E67" s="32" t="s">
         <v>139</v>
       </c>
-      <c r="F64" s="32" t="s">
+      <c r="F67" s="32" t="s">
         <v>140</v>
       </c>
-      <c r="G64" s="32" t="s">
+      <c r="G67" s="32" t="s">
         <v>141</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A65" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="B65" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="C65" s="32" t="s">
-        <v>70</v>
-      </c>
-      <c r="D65" s="32" t="s">
-        <v>70</v>
-      </c>
-      <c r="E65" s="32" t="s">
-        <v>70</v>
-      </c>
-      <c r="F65" s="32" t="s">
-        <v>70</v>
-      </c>
-      <c r="G65" s="32" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A66" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="B66" s="10">
-        <v>3.92</v>
-      </c>
-      <c r="C66" s="32">
-        <v>3.92</v>
-      </c>
-      <c r="D66" s="32">
-        <v>3.88</v>
-      </c>
-      <c r="E66" s="32">
-        <v>3.94</v>
-      </c>
-      <c r="F66" s="32">
-        <v>3.69</v>
-      </c>
-      <c r="G66" s="32">
-        <v>3.88</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>